<commit_message>
Added the modified / debugged server code to RasPiServer/
</commit_message>
<xml_diff>
--- a/Documents/Hardware/Power Supplies_phase2.xlsx
+++ b/Documents/Hardware/Power Supplies_phase2.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$B$2:$H$30</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Sheet2!$B$2:$H$31</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -337,12 +337,24 @@
   </si>
   <si>
     <t>shunt-tripped</t>
+  </si>
+  <si>
+    <t>Misc 2</t>
+  </si>
+  <si>
+    <t>Misc 1</t>
+  </si>
+  <si>
+    <t>Existing wall strips</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -485,7 +497,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -545,7 +557,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent1" xfId="4" builtinId="29"/>
@@ -1262,10 +1276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H30"/>
+  <dimension ref="B2:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="H31" sqref="B20:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,7 +1564,10 @@
       <c r="E21" t="s">
         <v>93</v>
       </c>
-      <c r="G21">
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" s="23">
         <f>C21*D21</f>
         <v>4160</v>
       </c>
@@ -1571,8 +1588,8 @@
       <c r="F22" t="s">
         <v>102</v>
       </c>
-      <c r="G22">
-        <f t="shared" ref="G22:G29" si="0">C22*D22</f>
+      <c r="G22" s="23">
+        <f t="shared" ref="G22:G30" si="0">C22*D22</f>
         <v>3328</v>
       </c>
     </row>
@@ -1592,7 +1609,7 @@
       <c r="F23" t="s">
         <v>102</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="23">
         <f t="shared" si="0"/>
         <v>3328</v>
       </c>
@@ -1610,7 +1627,10 @@
       <c r="E24" t="s">
         <v>96</v>
       </c>
-      <c r="G24">
+      <c r="F24" t="s">
+        <v>102</v>
+      </c>
+      <c r="G24" s="23">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
@@ -1628,7 +1648,7 @@
       <c r="E25" t="s">
         <v>97</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="23">
         <f t="shared" si="0"/>
         <v>1920</v>
       </c>
@@ -1646,7 +1666,7 @@
       <c r="E26" t="s">
         <v>90</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="23">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
@@ -1664,7 +1684,7 @@
       <c r="E27" t="s">
         <v>98</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="23">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
@@ -1682,7 +1702,7 @@
       <c r="E28" t="s">
         <v>99</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="23">
         <f t="shared" si="0"/>
         <v>2400</v>
       </c>
@@ -1698,7 +1718,10 @@
         <v>16</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>104</v>
+      </c>
+      <c r="F29" t="s">
+        <v>105</v>
       </c>
       <c r="G29" s="23">
         <f t="shared" si="0"/>
@@ -1706,11 +1729,32 @@
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="G30">
-        <f>SUM(G21:G29)/1000</f>
-        <v>23.776</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>120</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F30" t="s">
+        <v>105</v>
+      </c>
+      <c r="G30" s="24">
+        <f t="shared" si="0"/>
+        <v>1920</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G31" s="25">
+        <f>SUM(G21:G30)/1000</f>
+        <v>25.696000000000002</v>
+      </c>
+      <c r="H31" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>